<commit_message>
Update attendance list for fourth group
</commit_message>
<xml_diff>
--- a/lists/fourth-group.xlsx
+++ b/lists/fourth-group.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,16 +430,16 @@
       <selection activeCell="Q4" sqref="Q4:Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.7109375"/>
-    <col min="2" max="2" width="17.85546875"/>
+    <col min="1" max="1" width="46.6640625"/>
+    <col min="2" max="2" width="17.88671875"/>
     <col min="3" max="3" width="14"/>
-    <col min="4" max="15" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="21" width="12.5703125" customWidth="1"/>
+    <col min="4" max="15" width="12.5546875" hidden="1" customWidth="1"/>
+    <col min="16" max="21" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +504,7 @@
         <v>43251</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -515,7 +515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -526,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -570,7 +570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -617,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -673,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -717,7 +717,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -728,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -784,7 +784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -828,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -884,7 +884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -937,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -975,7 +975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -986,7 +986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -997,7 +997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>

</xml_diff>